<commit_message>
Updated CLR/OLRs for production ingest
</commit_message>
<xml_diff>
--- a/galactose/CLR/CLR_galactose.xlsx
+++ b/galactose/CLR/CLR_galactose.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\galactose\CLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\galactose_network_induction\CLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" tabRatio="365"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21990" windowHeight="6000" tabRatio="365"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="645">
   <si>
     <t>text</t>
   </si>
@@ -2071,12 +2071,6 @@
     <t>2016-12-31</t>
   </si>
   <si>
-    <t>Stockwell, Sarah R; Rifkin, Scott A (2017): Data from: A Living Vector Field Reveals Constraints on Galactose Network Induction in Yeast. UC San Diego Library Digital Collections.</t>
-  </si>
-  <si>
-    <t>Dynamics | Galactose | Gene expression | Single-cell | Yeast | Microscopy | Microfluidics | Time series</t>
-  </si>
-  <si>
     <t>Abstract: When a cell encounters a new environment, its transcriptional response can be constrained by its history. For example, yeast cells in galactose induce GAL genes with a speed and unanimity that depends on previous nutrient conditions. Cellular memory of long-term glucose exposure delays GAL induction and makes it highly variable with in a cell population, while other nutrient histories lead to rapid, uniform responses. To investigate how cell-level gene expression dynamics produce population-level phenotypes, we collected thousands of microscopy images of fields of cells as they switched to galactose from various nutrient histories, extracted time series of thousands of individual cells undergoing this shift, and used these to build living vector fields as the cells moved across the state space of the proteins Gal3p and Gal1p. We show that, after sustained glucose exposure, the lack of these GAL transducers leads to induction delays that are long but also variable; that cellular resources constrain induction; and that bimodally distributed expression levels arise from lineage selection - a subpopulation of cells induces more quickly and outcompetes the rest. Our results illuminate cellular memory in this important model system and illustrate how resources and randomness interact to shape the response of a population to a new environment.</t>
   </si>
   <si>
@@ -2087,6 +2081,21 @@
   </si>
   <si>
     <t>Data from: A Living Vector Field Reveals Constraints on Galactose Network Induction in Yeast</t>
+  </si>
+  <si>
+    <t>DC_Image.png</t>
+  </si>
+  <si>
+    <t>To study how cellular traits produce population phenotypes, we built living vector fields from single-cell timecourses of the proteins Gal3p and Gal1p as yeast switched to galactose from other nutrients. This collection has data and analysis codes.</t>
+  </si>
+  <si>
+    <t>Stockwell, Sarah R. and Rifkin, Scott A. 2017. A living vector field reveals constraints on galactose network induction in yeast. Molecular Systems Biology 13(908). http://doi.org/10.15252/msb.20167323</t>
+  </si>
+  <si>
+    <t>Stockwell, Sarah R; Rifkin, Scott A (2017): Data from: A Living Vector Field Reveals Constraints on Galactose Network Induction in Yeast. UC San Diego Library Digital Collections. https://doi.org/10.6075/J0C24TCX</t>
+  </si>
+  <si>
+    <t>Dynamics | Galactose | Gene expression | Single-cell organisms | Yeast | Microscopy | Microfluidics | Time series</t>
   </si>
 </sst>
 </file>
@@ -2324,7 +2333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2533,6 +2542,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -2718,7 +2733,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2771,6 +2786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3136,10 +3152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3153,12 +3169,12 @@
     <col min="8" max="8" width="14.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="39" style="3" customWidth="1"/>
-    <col min="11" max="12" width="39.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="42.85546875" style="3" customWidth="1"/>
-    <col min="14" max="15" width="84.28515625" style="3" customWidth="1"/>
+    <col min="11" max="13" width="39.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="42.85546875" style="3" customWidth="1"/>
+    <col min="15" max="16" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>336</v>
       </c>
@@ -3196,24 +3212,30 @@
         <v>3</v>
       </c>
       <c r="M1" s="16" t="s">
+        <v>628</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>481</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>630</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>640</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>356</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>631</v>
@@ -3230,24 +3252,30 @@
       <c r="I2" s="3" t="s">
         <v>635</v>
       </c>
+      <c r="J2" s="3" t="s">
+        <v>641</v>
+      </c>
       <c r="K2" s="23" t="s">
+        <v>643</v>
+      </c>
+      <c r="L2" s="23" t="s">
         <v>636</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="M2" s="26" t="s">
+        <v>642</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>640</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="C1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3255,7 +3283,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
@@ -3278,13 +3306,13 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>M1</xm:sqref>
+          <xm:sqref>N1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:O1</xm:sqref>
+          <xm:sqref>O1:P1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3296,7 +3324,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>K1:L1</xm:sqref>
+          <xm:sqref>K1:M1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>